<commit_message>
Detail base routines added, missing fields
</commit_message>
<xml_diff>
--- a/src/main/resources/plantilla-base-flujo.xlsx
+++ b/src/main/resources/plantilla-base-flujo.xlsx
@@ -4,11 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="23595" windowHeight="8700"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="23595" windowHeight="8700" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Base Flujo" sheetId="1" r:id="rId1"/>
+    <sheet name="Base Detalle" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="30">
   <si>
     <t>Punto de Venta</t>
   </si>
@@ -58,6 +58,55 @@
   </si>
   <si>
     <t>TIPO PDV</t>
+  </si>
+  <si>
+    <t>Persona Nº</t>
+  </si>
+  <si>
+    <t>Marca</t>
+  </si>
+  <si>
+    <t>Modelo</t>
+  </si>
+  <si>
+    <t>Tipo de Contrato</t>
+  </si>
+  <si>
+    <t>Modalidad de Equipo</t>
+  </si>
+  <si>
+    <t>Otras: Tarjeta</t>
+  </si>
+  <si>
+    <t>Otras: Chip</t>
+  </si>
+  <si>
+    <t>Otras: Accesorios</t>
+  </si>
+  <si>
+    <t>Calificación
+Plan</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>Calificación Equipo</t>
+  </si>
+  <si>
+    <t>Recarga Express</t>
+  </si>
+  <si>
+    <t>Carac Adicional</t>
+  </si>
+  <si>
+    <t>Total Ventas</t>
+  </si>
+  <si>
+    <t>Cambios Portabilidad</t>
+  </si>
+  <si>
+    <t>Razones Portabilidad</t>
   </si>
 </sst>
 </file>
@@ -99,7 +148,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -110,6 +159,12 @@
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="10"/>
+        <bgColor indexed="60"/>
       </patternFill>
     </fill>
   </fills>
@@ -129,13 +184,28 @@
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -444,7 +514,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -501,12 +571,92 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:25" ht="39" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="Y1" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>